<commit_message>
presi un sacco di dati venturi
</commit_message>
<xml_diff>
--- a/VENTURI/venturi_dati.xlsx
+++ b/VENTURI/venturi_dati.xlsx
@@ -62,10 +62,17 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,6 +602,9 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" s="1">
@@ -615,86 +625,528 @@
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="1">
-        <v>100.98999999999999</v>
+        <v>100.78</v>
       </c>
       <c r="B3" s="1">
-        <v>100.44</v>
+        <v>100.18000000000001</v>
       </c>
       <c r="C3" s="1">
-        <v>100.73</v>
+        <v>100.43000000000001</v>
       </c>
       <c r="D3" s="1">
-        <v>100.17</v>
+        <v>100.13</v>
       </c>
       <c r="E3" s="2">
-        <v>65</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="1">
-        <v>101.88</v>
+        <v>100.75</v>
       </c>
       <c r="B4" s="1">
-        <v>100.79000000000001</v>
+        <v>100.23999999999999</v>
       </c>
       <c r="C4" s="1">
-        <v>101.36</v>
+        <v>100.47</v>
       </c>
       <c r="D4" s="1">
-        <v>100.31999999999999</v>
+        <v>100.12</v>
       </c>
       <c r="E4" s="2">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="1">
-        <v>102.65000000000001</v>
+        <v>100.81999999999999</v>
       </c>
       <c r="B5" s="1">
-        <v>101.19</v>
+        <v>100.26000000000001</v>
       </c>
       <c r="C5" s="1">
-        <v>102.03</v>
+        <v>100.45</v>
       </c>
       <c r="D5" s="1">
-        <v>100.45</v>
+        <v>100.13</v>
       </c>
       <c r="E5" s="2">
-        <v>95</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="1">
-        <v>103.44</v>
+        <v>100.79000000000001</v>
       </c>
       <c r="B6" s="1">
-        <v>101.7</v>
+        <v>100.25</v>
       </c>
       <c r="C6" s="1">
-        <v>102.78</v>
+        <v>100.48</v>
       </c>
       <c r="D6" s="1">
-        <v>100.59</v>
+        <v>100.13</v>
       </c>
       <c r="E6" s="2">
-        <v>110</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" s="1">
+        <v>100.98999999999999</v>
+      </c>
+      <c r="B7" s="1">
+        <v>100.44</v>
+      </c>
+      <c r="C7" s="1">
+        <v>100.73</v>
+      </c>
+      <c r="D7" s="1">
+        <v>100.17</v>
+      </c>
+      <c r="E7" s="2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" s="1">
+        <v>101.18000000000001</v>
+      </c>
+      <c r="B8" s="1">
+        <v>100.45</v>
+      </c>
+      <c r="C8" s="1">
+        <v>100.81999999999999</v>
+      </c>
+      <c r="D8" s="1">
+        <v>100.19</v>
+      </c>
+      <c r="E8" s="2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" s="1">
+        <v>101.23</v>
+      </c>
+      <c r="B9" s="1">
+        <v>100.45</v>
+      </c>
+      <c r="C9" s="1">
+        <v>100.81999999999999</v>
+      </c>
+      <c r="D9" s="1">
+        <v>100.2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" s="1">
+        <v>100.93000000000001</v>
+      </c>
+      <c r="B10" s="1">
+        <v>100.36</v>
+      </c>
+      <c r="C10" s="1">
+        <v>100.77</v>
+      </c>
+      <c r="D10" s="1">
+        <v>100.15000000000001</v>
+      </c>
+      <c r="E10" s="2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11" s="1">
+        <v>101.01000000000001</v>
+      </c>
+      <c r="B11" s="1">
+        <v>100.37</v>
+      </c>
+      <c r="C11" s="1">
+        <v>100.68000000000001</v>
+      </c>
+      <c r="D11" s="1">
+        <v>100.16</v>
+      </c>
+      <c r="E11" s="2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="1">
+        <v>101.88</v>
+      </c>
+      <c r="B12" s="1">
+        <v>100.79000000000001</v>
+      </c>
+      <c r="C12" s="1">
+        <v>101.36</v>
+      </c>
+      <c r="D12" s="1">
+        <v>100.31999999999999</v>
+      </c>
+      <c r="E12" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13" s="1">
+        <v>101.86</v>
+      </c>
+      <c r="B13" s="1">
+        <v>100.73999999999999</v>
+      </c>
+      <c r="C13" s="1">
+        <v>101.33</v>
+      </c>
+      <c r="D13" s="1">
+        <v>100.3</v>
+      </c>
+      <c r="E13" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14" s="1">
+        <v>101.73</v>
+      </c>
+      <c r="B14" s="1">
+        <v>100.69</v>
+      </c>
+      <c r="C14" s="1">
+        <v>101.23</v>
+      </c>
+      <c r="D14" s="1">
+        <v>100.28</v>
+      </c>
+      <c r="E14" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15" s="1">
+        <v>101.53</v>
+      </c>
+      <c r="B15" s="1">
+        <v>100.65000000000001</v>
+      </c>
+      <c r="C15" s="1">
+        <v>101.12</v>
+      </c>
+      <c r="D15" s="1">
+        <v>100.25</v>
+      </c>
+      <c r="E15" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" s="1">
+        <v>101.88</v>
+      </c>
+      <c r="B16" s="1">
+        <v>100.73999999999999</v>
+      </c>
+      <c r="C16" s="1">
+        <v>101.33</v>
+      </c>
+      <c r="D16" s="1">
+        <v>100.3</v>
+      </c>
+      <c r="E16">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17" s="1">
+        <v>102.65000000000001</v>
+      </c>
+      <c r="B17" s="1">
+        <v>101.19</v>
+      </c>
+      <c r="C17" s="1">
+        <v>102.03</v>
+      </c>
+      <c r="D17" s="1">
+        <v>100.45</v>
+      </c>
+      <c r="E17" s="2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="A18" s="1">
+        <v>103.09999999999999</v>
+      </c>
+      <c r="B18" s="1">
+        <v>101.36</v>
+      </c>
+      <c r="C18" s="1">
+        <v>102.34999999999999</v>
+      </c>
+      <c r="D18" s="1">
+        <v>100.51000000000001</v>
+      </c>
+      <c r="E18" s="2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="A19" s="1">
+        <v>103.3</v>
+      </c>
+      <c r="B19" s="1">
+        <v>101.45</v>
+      </c>
+      <c r="C19" s="1">
+        <v>102.51000000000001</v>
+      </c>
+      <c r="D19" s="1">
+        <v>100.55</v>
+      </c>
+      <c r="E19" s="2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="A20" s="1">
+        <v>102.40000000000001</v>
+      </c>
+      <c r="B20" s="1">
+        <v>101.13</v>
+      </c>
+      <c r="C20" s="1">
+        <v>101.89</v>
+      </c>
+      <c r="D20" s="1">
+        <v>100.40000000000001</v>
+      </c>
+      <c r="E20">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21" s="1">
+        <v>102.91</v>
+      </c>
+      <c r="B21" s="1">
+        <v>101.31</v>
+      </c>
+      <c r="C21" s="1">
+        <v>102.22</v>
+      </c>
+      <c r="D21" s="1">
+        <v>100.48</v>
+      </c>
+      <c r="E21">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="A22" s="3">
+        <v>102.87</v>
+      </c>
+      <c r="B22" s="3">
+        <v>101.34999999999999</v>
+      </c>
+      <c r="C22" s="3">
+        <v>102.25</v>
+      </c>
+      <c r="D22" s="3">
+        <v>100.47</v>
+      </c>
+      <c r="E22" s="4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="A23" s="3">
+        <v>102.77</v>
+      </c>
+      <c r="B23" s="3">
+        <v>101.31999999999999</v>
+      </c>
+      <c r="C23" s="3">
+        <v>102.2</v>
+      </c>
+      <c r="D23" s="3">
+        <v>100.45999999999999</v>
+      </c>
+      <c r="E23" s="4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="A24" s="1">
+        <v>103.44</v>
+      </c>
+      <c r="B24" s="1">
+        <v>101.7</v>
+      </c>
+      <c r="C24" s="1">
+        <v>102.78</v>
+      </c>
+      <c r="D24" s="1">
+        <v>100.59</v>
+      </c>
+      <c r="E24" s="2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="A25" s="1">
+        <v>103.90000000000001</v>
+      </c>
+      <c r="B25" s="1">
+        <v>101.76000000000001</v>
+      </c>
+      <c r="C25" s="1">
+        <v>103.01000000000001</v>
+      </c>
+      <c r="D25" s="1">
+        <v>100.66</v>
+      </c>
+      <c r="E25" s="2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="A26" s="3">
+        <v>104.20999999999999</v>
+      </c>
+      <c r="B26" s="3">
+        <v>101.95</v>
+      </c>
+      <c r="C26" s="3">
+        <v>103.31999999999999</v>
+      </c>
+      <c r="D26" s="3">
+        <v>100.70999999999999</v>
+      </c>
+      <c r="E26" s="5">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="A27" s="3">
+        <v>104.42</v>
+      </c>
+      <c r="B27" s="3">
+        <v>102.04000000000001</v>
+      </c>
+      <c r="C27" s="3">
+        <v>103.48999999999999</v>
+      </c>
+      <c r="D27" s="3">
+        <v>100.76000000000001</v>
+      </c>
+      <c r="E27" s="5">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25">
+      <c r="A28" s="3">
+        <v>104.25</v>
+      </c>
+      <c r="B28" s="3">
+        <v>101.95</v>
+      </c>
+      <c r="C28" s="3">
+        <v>103.34</v>
+      </c>
+      <c r="D28" s="3">
+        <v>100.72</v>
+      </c>
+      <c r="E28" s="5">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" ht="14.25">
+      <c r="A29" s="1">
         <v>104.61</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B29" s="1">
         <v>102.2</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C29" s="1">
         <v>103.73</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D29" s="1">
         <v>100.81999999999999</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E29" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25">
+      <c r="A30" s="3">
+        <v>104.59</v>
+      </c>
+      <c r="B30" s="3">
+        <v>102.18000000000001</v>
+      </c>
+      <c r="C30" s="3">
+        <v>103.65000000000001</v>
+      </c>
+      <c r="D30" s="3">
+        <v>100.78</v>
+      </c>
+      <c r="E30" s="5">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" ht="14.25">
+      <c r="A31" s="3">
+        <v>105.23999999999999</v>
+      </c>
+      <c r="B31" s="3">
+        <v>102.52</v>
+      </c>
+      <c r="C31" s="3">
+        <v>104.23999999999999</v>
+      </c>
+      <c r="D31" s="3">
+        <v>100.93000000000001</v>
+      </c>
+      <c r="E31" s="5">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" ht="14.25">
+      <c r="A32" s="3">
+        <v>104.62</v>
+      </c>
+      <c r="B32" s="3">
+        <v>102.23999999999999</v>
+      </c>
+      <c r="C32" s="3">
+        <v>103.73</v>
+      </c>
+      <c r="D32" s="3">
+        <v>100.8</v>
+      </c>
+      <c r="E32" s="5">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" ht="14.25">
+      <c r="A33" s="3">
+        <v>104.89</v>
+      </c>
+      <c r="B33" s="3">
+        <v>102.31</v>
+      </c>
+      <c r="C33" s="3">
+        <v>103.91</v>
+      </c>
+      <c r="D33" s="3">
+        <v>100.84999999999999</v>
+      </c>
+      <c r="E33" s="5">
         <v>125</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rifatte misure e senza saper scrivere ne leggere assunta una deviazione standard che sovrastima l'errore
</commit_message>
<xml_diff>
--- a/VENTURI/venturi_dati.xlsx
+++ b/VENTURI/venturi_dati.xlsx
@@ -3,17 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ARIA" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="ARIA TRA I 10 E 60 lmin-1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>p1</t>
   </si>
@@ -28,12 +29,54 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>p1m</t>
+  </si>
+  <si>
+    <t>p2m</t>
+  </si>
+  <si>
+    <t>p3m</t>
+  </si>
+  <si>
+    <t>p4m</t>
+  </si>
+  <si>
+    <t>Rm</t>
+  </si>
+  <si>
+    <t>STD1</t>
+  </si>
+  <si>
+    <t>STD2</t>
+  </si>
+  <si>
+    <t>STD3</t>
+  </si>
+  <si>
+    <t>STD4</t>
+  </si>
+  <si>
+    <t>offset1</t>
+  </si>
+  <si>
+    <t>offset2</t>
+  </si>
+  <si>
+    <t>offset3</t>
+  </si>
+  <si>
+    <t>offset4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="160" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11.000000"/>
@@ -62,10 +105,12 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -580,7 +625,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -603,7 +648,43 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" ht="14.25">
@@ -622,6 +703,53 @@
       <c r="E2" s="2">
         <v>50</v>
       </c>
+      <c r="F2" s="1">
+        <f>AVERAGE(A2:A6)</f>
+        <v>100.76000000000001</v>
+      </c>
+      <c r="G2" s="1">
+        <f>AVERAGE(B2:B6)</f>
+        <v>100.25</v>
+      </c>
+      <c r="H2" s="1">
+        <f>AVERAGE(C2:C6)</f>
+        <v>100.462</v>
+      </c>
+      <c r="I2" s="1">
+        <f>AVERAGE(D2:D6)</f>
+        <v>100.126</v>
+      </c>
+      <c r="J2">
+        <v>50</v>
+      </c>
+      <c r="K2" s="1">
+        <f>STDEV(A2:A6)</f>
+        <v>0.061237243569580033</v>
+      </c>
+      <c r="L2" s="3">
+        <f>STDEV(B2:B6)</f>
+        <v>0.049999999999995735</v>
+      </c>
+      <c r="M2" s="3">
+        <f>STDEV(C2:C6)</f>
+        <v>0.021679483388677437</v>
+      </c>
+      <c r="N2" s="3">
+        <f>STDEV(D2:D6)</f>
+        <v>0.0054772255750466792</v>
+      </c>
+      <c r="O2" s="4">
+        <v>0.249</v>
+      </c>
+      <c r="P2" s="4">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="R2" s="4">
+        <v>0.29999999999999999</v>
+      </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="1">
@@ -639,6 +767,41 @@
       <c r="E3" s="2">
         <v>50</v>
       </c>
+      <c r="F3" s="1">
+        <f>AVERAGE(A7:A11)</f>
+        <v>101.06800000000001</v>
+      </c>
+      <c r="G3" s="1">
+        <f>AVERAGE(B7:B11)</f>
+        <v>100.414</v>
+      </c>
+      <c r="H3" s="1">
+        <f>AVERAGE(C7:C11)</f>
+        <v>100.764</v>
+      </c>
+      <c r="I3" s="1">
+        <f>AVERAGE(D7:D11)</f>
+        <v>100.17400000000001</v>
+      </c>
+      <c r="J3">
+        <v>65</v>
+      </c>
+      <c r="K3" s="1">
+        <f>STDEV(A7:A11)</f>
+        <v>0.1296919426949889</v>
+      </c>
+      <c r="L3" s="3">
+        <f>STDEV(B7:B11)</f>
+        <v>0.045055521304275106</v>
+      </c>
+      <c r="M3" s="3">
+        <f>STDEV(C7:C11)</f>
+        <v>0.060249481325562064</v>
+      </c>
+      <c r="N3" s="3">
+        <f>STDEV(D7:D11)</f>
+        <v>0.020736441353327022</v>
+      </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="1">
@@ -656,6 +819,41 @@
       <c r="E4" s="2">
         <v>50</v>
       </c>
+      <c r="F4" s="1">
+        <f>AVERAGE(A12:A16)</f>
+        <v>101.776</v>
+      </c>
+      <c r="G4" s="1">
+        <f>AVERAGE(B12:B16)</f>
+        <v>100.72200000000001</v>
+      </c>
+      <c r="H4" s="1">
+        <f>AVERAGE(C12:C16)</f>
+        <v>101.274</v>
+      </c>
+      <c r="I4" s="1">
+        <f>AVERAGE(D12:D16)</f>
+        <v>100.28999999999999</v>
+      </c>
+      <c r="J4">
+        <v>80</v>
+      </c>
+      <c r="K4" s="1">
+        <f>STDEV(A12:A16)</f>
+        <v>0.15109599597606574</v>
+      </c>
+      <c r="L4" s="3">
+        <f>STDEV(B12:B16)</f>
+        <v>0.053572380943915053</v>
+      </c>
+      <c r="M4" s="3">
+        <f>STDEV(C12:C16)</f>
+        <v>0.099146356463560695</v>
+      </c>
+      <c r="N4" s="3">
+        <f>STDEV(D12:D16)</f>
+        <v>0.02645751311064333</v>
+      </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="1">
@@ -673,6 +871,41 @@
       <c r="E5" s="2">
         <v>50</v>
       </c>
+      <c r="F5" s="1">
+        <f>AVERAGE(A17:A21)</f>
+        <v>102.98999999999998</v>
+      </c>
+      <c r="G5" s="1">
+        <f>AVERAGE(B17:B21)</f>
+        <v>101.358</v>
+      </c>
+      <c r="H5" s="1">
+        <f>AVERAGE(C17:C21)</f>
+        <v>102.30600000000001</v>
+      </c>
+      <c r="I5" s="1">
+        <f>AVERAGE(D17:D21)</f>
+        <v>100.494</v>
+      </c>
+      <c r="J5">
+        <v>95</v>
+      </c>
+      <c r="K5" s="1">
+        <f>STDEV((A17:A21))</f>
+        <v>0.21059439688652581</v>
+      </c>
+      <c r="L5" s="3">
+        <f>STDEV((B17:B21))</f>
+        <v>0.055407580708782336</v>
+      </c>
+      <c r="M5" s="3">
+        <f>STDEV((C17:C21))</f>
+        <v>0.12778888840584027</v>
+      </c>
+      <c r="N5" s="3">
+        <f>STDEV((D17:D21))</f>
+        <v>0.036469165057621669</v>
+      </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="1">
@@ -690,6 +923,41 @@
       <c r="E6" s="2">
         <v>50</v>
       </c>
+      <c r="F6" s="1">
+        <f>AVERAGE(A22:A26)</f>
+        <v>104.04400000000001</v>
+      </c>
+      <c r="G6" s="1">
+        <f>AVERAGE(B22:B26)</f>
+        <v>101.88000000000001</v>
+      </c>
+      <c r="H6" s="1">
+        <f>AVERAGE(C22:C26)</f>
+        <v>103.18800000000002</v>
+      </c>
+      <c r="I6" s="1">
+        <f>AVERAGE(D22:D26)</f>
+        <v>100.68799999999999</v>
+      </c>
+      <c r="J6">
+        <v>110</v>
+      </c>
+      <c r="K6" s="1">
+        <f>STDEV((A22:A26))</f>
+        <v>0.386302989892649</v>
+      </c>
+      <c r="L6" s="3">
+        <f>STDEV((B22:B26))</f>
+        <v>0.143352711868315</v>
+      </c>
+      <c r="M6" s="3">
+        <f>STDEV((C22:C26))</f>
+        <v>0.287175904281676</v>
+      </c>
+      <c r="N6" s="3">
+        <f>STDEV((D22:D26))</f>
+        <v>0.065345237010818</v>
+      </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" s="1">
@@ -707,6 +975,41 @@
       <c r="E7" s="2">
         <v>65</v>
       </c>
+      <c r="F7" s="1">
+        <f>AVERAGE(A27:A31)</f>
+        <v>104.79000000000001</v>
+      </c>
+      <c r="G7" s="1">
+        <f>AVERAGE(B27:B31)</f>
+        <v>102.28999999999999</v>
+      </c>
+      <c r="H7" s="1">
+        <f>AVERAGE(C27:C31)</f>
+        <v>103.852</v>
+      </c>
+      <c r="I7" s="1">
+        <f>AVERAGE(D27:D31)</f>
+        <v>100.83599999999998</v>
+      </c>
+      <c r="J7">
+        <v>125</v>
+      </c>
+      <c r="K7" s="1">
+        <f>STDEV((A27:A31))</f>
+        <v>0.28008927148321516</v>
+      </c>
+      <c r="L7" s="3">
+        <f>STDEV((B27:B31))</f>
+        <v>0.13784048752089928</v>
+      </c>
+      <c r="M7" s="3">
+        <f>STDEV((C27:C31))</f>
+        <v>0.23689660191737205</v>
+      </c>
+      <c r="N7" s="3">
+        <f>STDEV((D27:D31))</f>
+        <v>0.058566201857388318</v>
+      </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="1">
@@ -863,16 +1166,16 @@
     </row>
     <row r="17" ht="14.25">
       <c r="A17" s="1">
-        <v>102.65000000000001</v>
+        <v>103.09999999999999</v>
       </c>
       <c r="B17" s="1">
-        <v>101.19</v>
+        <v>101.36</v>
       </c>
       <c r="C17" s="1">
-        <v>102.03</v>
+        <v>102.34999999999999</v>
       </c>
       <c r="D17" s="1">
-        <v>100.45</v>
+        <v>100.51000000000001</v>
       </c>
       <c r="E17" s="2">
         <v>95</v>
@@ -880,16 +1183,16 @@
     </row>
     <row r="18" ht="14.25">
       <c r="A18" s="1">
-        <v>103.09999999999999</v>
+        <v>103.3</v>
       </c>
       <c r="B18" s="1">
-        <v>101.36</v>
+        <v>101.45</v>
       </c>
       <c r="C18" s="1">
-        <v>102.34999999999999</v>
+        <v>102.51000000000001</v>
       </c>
       <c r="D18" s="1">
-        <v>100.51000000000001</v>
+        <v>100.55</v>
       </c>
       <c r="E18" s="2">
         <v>95</v>
@@ -897,259 +1200,328 @@
     </row>
     <row r="19" ht="14.25">
       <c r="A19" s="1">
-        <v>103.3</v>
+        <v>102.91</v>
       </c>
       <c r="B19" s="1">
-        <v>101.45</v>
+        <v>101.31</v>
       </c>
       <c r="C19" s="1">
-        <v>102.51000000000001</v>
+        <v>102.22</v>
       </c>
       <c r="D19" s="1">
-        <v>100.55</v>
-      </c>
-      <c r="E19" s="2">
+        <v>100.48</v>
+      </c>
+      <c r="E19">
         <v>95</v>
       </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="1">
-        <v>102.40000000000001</v>
-      </c>
-      <c r="B20" s="1">
-        <v>101.13</v>
-      </c>
-      <c r="C20" s="1">
-        <v>101.89</v>
-      </c>
-      <c r="D20" s="1">
-        <v>100.40000000000001</v>
-      </c>
-      <c r="E20">
+      <c r="A20" s="5">
+        <v>102.87</v>
+      </c>
+      <c r="B20" s="5">
+        <v>101.34999999999999</v>
+      </c>
+      <c r="C20" s="5">
+        <v>102.25</v>
+      </c>
+      <c r="D20" s="5">
+        <v>100.47</v>
+      </c>
+      <c r="E20" s="6">
         <v>95</v>
       </c>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="1">
-        <v>102.91</v>
-      </c>
-      <c r="B21" s="1">
-        <v>101.31</v>
-      </c>
-      <c r="C21" s="1">
-        <v>102.22</v>
-      </c>
-      <c r="D21" s="1">
-        <v>100.48</v>
-      </c>
-      <c r="E21">
+      <c r="A21" s="5">
+        <v>102.77</v>
+      </c>
+      <c r="B21" s="5">
+        <v>101.31999999999999</v>
+      </c>
+      <c r="C21" s="5">
+        <v>102.2</v>
+      </c>
+      <c r="D21" s="5">
+        <v>100.45999999999999</v>
+      </c>
+      <c r="E21" s="6">
         <v>95</v>
       </c>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="3">
-        <v>102.87</v>
-      </c>
-      <c r="B22" s="3">
-        <v>101.34999999999999</v>
-      </c>
-      <c r="C22" s="3">
-        <v>102.25</v>
-      </c>
-      <c r="D22" s="3">
-        <v>100.47</v>
-      </c>
-      <c r="E22" s="4">
-        <v>95</v>
+      <c r="A22" s="1">
+        <v>103.44</v>
+      </c>
+      <c r="B22" s="1">
+        <v>101.7</v>
+      </c>
+      <c r="C22" s="1">
+        <v>102.78</v>
+      </c>
+      <c r="D22" s="1">
+        <v>100.59</v>
+      </c>
+      <c r="E22" s="2">
+        <v>110</v>
       </c>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="3">
-        <v>102.77</v>
-      </c>
-      <c r="B23" s="3">
-        <v>101.31999999999999</v>
-      </c>
-      <c r="C23" s="3">
+      <c r="A23" s="1">
+        <v>103.90000000000001</v>
+      </c>
+      <c r="B23" s="1">
+        <v>101.76000000000001</v>
+      </c>
+      <c r="C23" s="1">
+        <v>103.01000000000001</v>
+      </c>
+      <c r="D23" s="1">
+        <v>100.66</v>
+      </c>
+      <c r="E23" s="2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="A24" s="5">
+        <v>104.20999999999999</v>
+      </c>
+      <c r="B24" s="5">
+        <v>101.95</v>
+      </c>
+      <c r="C24" s="5">
+        <v>103.31999999999999</v>
+      </c>
+      <c r="D24" s="5">
+        <v>100.70999999999999</v>
+      </c>
+      <c r="E24" s="7">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="A25" s="5">
+        <v>104.42</v>
+      </c>
+      <c r="B25" s="5">
+        <v>102.04000000000001</v>
+      </c>
+      <c r="C25" s="5">
+        <v>103.48999999999999</v>
+      </c>
+      <c r="D25" s="5">
+        <v>100.76000000000001</v>
+      </c>
+      <c r="E25" s="7">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="A26" s="5">
+        <v>104.25</v>
+      </c>
+      <c r="B26" s="5">
+        <v>101.95</v>
+      </c>
+      <c r="C26" s="5">
+        <v>103.34</v>
+      </c>
+      <c r="D26" s="5">
+        <v>100.72</v>
+      </c>
+      <c r="E26" s="7">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="A27" s="1">
+        <v>104.61</v>
+      </c>
+      <c r="B27" s="1">
         <v>102.2</v>
       </c>
-      <c r="D23" s="3">
-        <v>100.45999999999999</v>
-      </c>
-      <c r="E23" s="4">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" ht="14.25">
-      <c r="A24" s="1">
-        <v>103.44</v>
-      </c>
-      <c r="B24" s="1">
-        <v>101.7</v>
-      </c>
-      <c r="C24" s="1">
-        <v>102.78</v>
-      </c>
-      <c r="D24" s="1">
-        <v>100.59</v>
-      </c>
-      <c r="E24" s="2">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" ht="14.25">
-      <c r="A25" s="1">
-        <v>103.90000000000001</v>
-      </c>
-      <c r="B25" s="1">
-        <v>101.76000000000001</v>
-      </c>
-      <c r="C25" s="1">
-        <v>103.01000000000001</v>
-      </c>
-      <c r="D25" s="1">
-        <v>100.66</v>
-      </c>
-      <c r="E25" s="2">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" ht="14.25">
-      <c r="A26" s="3">
-        <v>104.20999999999999</v>
-      </c>
-      <c r="B26" s="3">
-        <v>101.95</v>
-      </c>
-      <c r="C26" s="3">
-        <v>103.31999999999999</v>
-      </c>
-      <c r="D26" s="3">
-        <v>100.70999999999999</v>
-      </c>
-      <c r="E26" s="5">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" ht="14.25">
-      <c r="A27" s="3">
-        <v>104.42</v>
-      </c>
-      <c r="B27" s="3">
-        <v>102.04000000000001</v>
-      </c>
-      <c r="C27" s="3">
-        <v>103.48999999999999</v>
-      </c>
-      <c r="D27" s="3">
+      <c r="C27" s="1">
+        <v>103.73</v>
+      </c>
+      <c r="D27" s="1">
+        <v>100.81999999999999</v>
+      </c>
+      <c r="E27" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25">
+      <c r="A28" s="5">
+        <v>104.59</v>
+      </c>
+      <c r="B28" s="5">
+        <v>102.18000000000001</v>
+      </c>
+      <c r="C28" s="5">
+        <v>103.65000000000001</v>
+      </c>
+      <c r="D28" s="5">
+        <v>100.78</v>
+      </c>
+      <c r="E28" s="7">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" ht="14.25">
+      <c r="A29" s="5">
+        <v>105.23999999999999</v>
+      </c>
+      <c r="B29" s="5">
+        <v>102.52</v>
+      </c>
+      <c r="C29" s="5">
+        <v>104.23999999999999</v>
+      </c>
+      <c r="D29" s="5">
+        <v>100.93000000000001</v>
+      </c>
+      <c r="E29" s="7">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25">
+      <c r="A30" s="5">
+        <v>104.62</v>
+      </c>
+      <c r="B30" s="5">
+        <v>102.23999999999999</v>
+      </c>
+      <c r="C30" s="5">
+        <v>103.73</v>
+      </c>
+      <c r="D30" s="5">
+        <v>100.8</v>
+      </c>
+      <c r="E30" s="7">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" ht="14.25">
+      <c r="A31" s="5">
+        <v>104.89</v>
+      </c>
+      <c r="B31" s="5">
+        <v>102.31</v>
+      </c>
+      <c r="C31" s="5">
+        <v>103.91</v>
+      </c>
+      <c r="D31" s="5">
+        <v>100.84999999999999</v>
+      </c>
+      <c r="E31" s="7">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>100.09</v>
+      </c>
+      <c r="B2" s="1">
+        <v>100.01000000000001</v>
+      </c>
+      <c r="C2" s="1">
+        <v>100.09999999999999</v>
+      </c>
+      <c r="D2" s="1">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>100.39</v>
+      </c>
+      <c r="B3" s="1">
+        <v>100.09999999999999</v>
+      </c>
+      <c r="C3" s="1">
+        <v>100.22</v>
+      </c>
+      <c r="D3" s="1">
+        <v>100.05</v>
+      </c>
+      <c r="E3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
         <v>100.76000000000001</v>
       </c>
-      <c r="E27" s="5">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" ht="14.25">
-      <c r="A28" s="3">
-        <v>104.25</v>
-      </c>
-      <c r="B28" s="3">
-        <v>101.95</v>
-      </c>
-      <c r="C28" s="3">
-        <v>103.34</v>
-      </c>
-      <c r="D28" s="3">
-        <v>100.72</v>
-      </c>
-      <c r="E28" s="5">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" ht="14.25">
-      <c r="A29" s="1">
-        <v>104.61</v>
-      </c>
-      <c r="B29" s="1">
-        <v>102.2</v>
-      </c>
-      <c r="C29" s="1">
-        <v>103.73</v>
-      </c>
-      <c r="D29" s="1">
-        <v>100.81999999999999</v>
-      </c>
-      <c r="E29" s="2">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="30" ht="14.25">
-      <c r="A30" s="3">
-        <v>104.59</v>
-      </c>
-      <c r="B30" s="3">
-        <v>102.18000000000001</v>
-      </c>
-      <c r="C30" s="3">
-        <v>103.65000000000001</v>
-      </c>
-      <c r="D30" s="3">
-        <v>100.78</v>
-      </c>
-      <c r="E30" s="5">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="31" ht="14.25">
-      <c r="A31" s="3">
-        <v>105.23999999999999</v>
-      </c>
-      <c r="B31" s="3">
-        <v>102.52</v>
-      </c>
-      <c r="C31" s="3">
-        <v>104.23999999999999</v>
-      </c>
-      <c r="D31" s="3">
-        <v>100.93000000000001</v>
-      </c>
-      <c r="E31" s="5">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="32" ht="14.25">
-      <c r="A32" s="3">
-        <v>104.62</v>
-      </c>
-      <c r="B32" s="3">
-        <v>102.23999999999999</v>
-      </c>
-      <c r="C32" s="3">
-        <v>103.73</v>
-      </c>
-      <c r="D32" s="3">
-        <v>100.8</v>
-      </c>
-      <c r="E32" s="5">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="33" ht="14.25">
-      <c r="A33" s="3">
-        <v>104.89</v>
-      </c>
-      <c r="B33" s="3">
-        <v>102.31</v>
-      </c>
-      <c r="C33" s="3">
-        <v>103.91</v>
-      </c>
-      <c r="D33" s="3">
-        <v>100.84999999999999</v>
-      </c>
-      <c r="E33" s="5">
-        <v>125</v>
-      </c>
-    </row>
+      <c r="B4" s="1">
+        <v>100.25</v>
+      </c>
+      <c r="C4" s="1">
+        <v>100.462</v>
+      </c>
+      <c r="D4" s="1">
+        <v>100.126</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>101.06800000000001</v>
+      </c>
+      <c r="B5" s="1">
+        <v>100.414</v>
+      </c>
+      <c r="C5" s="1">
+        <v>100.764</v>
+      </c>
+      <c r="D5" s="1">
+        <v>100.17400000000001</v>
+      </c>
+      <c r="E5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
i dati presi non sono buoni per nulla
</commit_message>
<xml_diff>
--- a/VENTURI/venturi_dati.xlsx
+++ b/VENTURI/venturi_dati.xlsx
@@ -7,14 +7,15 @@
   </bookViews>
   <sheets>
     <sheet name="ARIA" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="ARIA TRA I 10 E 60 lmin-1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="ACQUA" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="ARIA TRA I 10 E 60 lmin-1" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>p1</t>
   </si>
@@ -68,6 +69,24 @@
   </si>
   <si>
     <t>offset4</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>m_lorda</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>m_bottiglia</t>
+  </si>
+  <si>
+    <t>t</t>
   </si>
 </sst>
 </file>
@@ -105,11 +124,10 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1">
       <protection hidden="0" locked="1"/>
@@ -726,28 +744,28 @@
         <f>STDEV(A2:A6)</f>
         <v>0.061237243569580033</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="1">
         <f>STDEV(B2:B6)</f>
         <v>0.049999999999995735</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="1">
         <f>STDEV(C2:C6)</f>
         <v>0.021679483388677437</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="1">
         <f>STDEV(D2:D6)</f>
         <v>0.0054772255750466792</v>
       </c>
-      <c r="O2" s="4">
+      <c r="O2" s="3">
         <v>0.249</v>
       </c>
-      <c r="P2" s="4">
+      <c r="P2" s="3">
         <v>0.16600000000000001</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="Q2" s="3">
         <v>0.19800000000000001</v>
       </c>
-      <c r="R2" s="4">
+      <c r="R2" s="3">
         <v>0.29999999999999999</v>
       </c>
     </row>
@@ -790,15 +808,15 @@
         <f>STDEV(A7:A11)</f>
         <v>0.1296919426949889</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="1">
         <f>STDEV(B7:B11)</f>
         <v>0.045055521304275106</v>
       </c>
-      <c r="M3" s="3">
+      <c r="M3" s="1">
         <f>STDEV(C7:C11)</f>
         <v>0.060249481325562064</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3" s="1">
         <f>STDEV(D7:D11)</f>
         <v>0.020736441353327022</v>
       </c>
@@ -842,15 +860,15 @@
         <f>STDEV(A12:A16)</f>
         <v>0.15109599597606574</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="1">
         <f>STDEV(B12:B16)</f>
         <v>0.053572380943915053</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="1">
         <f>STDEV(C12:C16)</f>
         <v>0.099146356463560695</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="1">
         <f>STDEV(D12:D16)</f>
         <v>0.02645751311064333</v>
       </c>
@@ -894,15 +912,15 @@
         <f>STDEV((A17:A21))</f>
         <v>0.21059439688652581</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="1">
         <f>STDEV((B17:B21))</f>
         <v>0.055407580708782336</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5" s="1">
         <f>STDEV((C17:C21))</f>
         <v>0.12778888840584027</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="1">
         <f>STDEV((D17:D21))</f>
         <v>0.036469165057621669</v>
       </c>
@@ -946,15 +964,15 @@
         <f>STDEV((A22:A26))</f>
         <v>0.386302989892649</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="1">
         <f>STDEV((B22:B26))</f>
         <v>0.143352711868315</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M6" s="1">
         <f>STDEV((C22:C26))</f>
         <v>0.287175904281676</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="1">
         <f>STDEV((D22:D26))</f>
         <v>0.065345237010818</v>
       </c>
@@ -998,15 +1016,15 @@
         <f>STDEV((A27:A31))</f>
         <v>0.28008927148321516</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="1">
         <f>STDEV((B27:B31))</f>
         <v>0.13784048752089928</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M7" s="1">
         <f>STDEV((C27:C31))</f>
         <v>0.23689660191737205</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="1">
         <f>STDEV((D27:D31))</f>
         <v>0.058566201857388318</v>
       </c>
@@ -1216,36 +1234,36 @@
       </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="5">
+      <c r="A20" s="4">
         <v>102.87</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="4">
         <v>101.34999999999999</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <v>102.25</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <v>100.47</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>95</v>
       </c>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="5">
+      <c r="A21" s="4">
         <v>102.77</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="4">
         <v>101.31999999999999</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="4">
         <v>102.2</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="4">
         <v>100.45999999999999</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>95</v>
       </c>
     </row>
@@ -1284,53 +1302,53 @@
       </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="5">
+      <c r="A24" s="4">
         <v>104.20999999999999</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="4">
         <v>101.95</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <v>103.31999999999999</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="4">
         <v>100.70999999999999</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="6">
         <v>110</v>
       </c>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" s="5">
+      <c r="A25" s="4">
         <v>104.42</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="4">
         <v>102.04000000000001</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <v>103.48999999999999</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="4">
         <v>100.76000000000001</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="6">
         <v>110</v>
       </c>
     </row>
     <row r="26" ht="14.25">
-      <c r="A26" s="5">
+      <c r="A26" s="4">
         <v>104.25</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="4">
         <v>101.95</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="4">
         <v>103.34</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="4">
         <v>100.72</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="6">
         <v>110</v>
       </c>
     </row>
@@ -1352,70 +1370,70 @@
       </c>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="5">
+      <c r="A28" s="4">
         <v>104.59</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="4">
         <v>102.18000000000001</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="4">
         <v>103.65000000000001</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="4">
         <v>100.78</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="6">
         <v>125</v>
       </c>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="5">
+      <c r="A29" s="4">
         <v>105.23999999999999</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="4">
         <v>102.52</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="4">
         <v>104.23999999999999</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="4">
         <v>100.93000000000001</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="6">
         <v>125</v>
       </c>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" s="5">
+      <c r="A30" s="4">
         <v>104.62</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="4">
         <v>102.23999999999999</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="4">
         <v>103.73</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="4">
         <v>100.8</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="6">
         <v>125</v>
       </c>
     </row>
     <row r="31" ht="14.25">
-      <c r="A31" s="5">
+      <c r="A31" s="4">
         <v>104.89</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="4">
         <v>102.31</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="4">
         <v>103.91</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="4">
         <v>100.84999999999999</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="6">
         <v>125</v>
       </c>
     </row>
@@ -1434,7 +1452,242 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col bestFit="1" min="10" max="10" width="10.5234375"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="C2" s="3">
+        <f t="shared" ref="C2:C6" si="0">B2-$J$2</f>
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D6" si="1">C2*1/1000</f>
+        <v>0.00061600000000000001</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E6" si="2">D2/$K$2</f>
+        <v>6.1600000000000007e-05</v>
+      </c>
+      <c r="F2" s="1">
+        <v>111.58</v>
+      </c>
+      <c r="G2" s="1">
+        <v>109.98999999999999</v>
+      </c>
+      <c r="H2" s="1">
+        <v>110.39</v>
+      </c>
+      <c r="I2" s="1">
+        <v>108.88</v>
+      </c>
+      <c r="J2">
+        <v>0.088999999999999996</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="C3" s="3">
+        <f t="shared" si="0"/>
+        <v>0.29500000000000004</v>
+      </c>
+      <c r="D3" s="5">
+        <f t="shared" si="1"/>
+        <v>0.00029500000000000001</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="2"/>
+        <v>2.9500000000000002e-05</v>
+      </c>
+      <c r="F3" s="1">
+        <v>103.52</v>
+      </c>
+      <c r="G3" s="1">
+        <v>102.97</v>
+      </c>
+      <c r="H3" s="1">
+        <v>103.34999999999999</v>
+      </c>
+      <c r="I3" s="1">
+        <v>102.65000000000001</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.44000000000000006</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" si="1"/>
+        <v>0.00044000000000000007</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000006e-05</v>
+      </c>
+      <c r="F4" s="1">
+        <v>121.29000000000001</v>
+      </c>
+      <c r="G4" s="1">
+        <v>118.33</v>
+      </c>
+      <c r="H4" s="1">
+        <v>119.48</v>
+      </c>
+      <c r="I4" s="1">
+        <v>116.31</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.495</v>
+      </c>
+      <c r="D5" s="5">
+        <f t="shared" si="1"/>
+        <v>0.000495</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>4.9499999999999997e-05</v>
+      </c>
+      <c r="F5" s="1">
+        <v>104.25</v>
+      </c>
+      <c r="G5" s="1">
+        <v>103.43000000000001</v>
+      </c>
+      <c r="H5" s="1">
+        <v>103.68000000000001</v>
+      </c>
+      <c r="I5" s="1">
+        <v>102.7</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.748</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" si="1"/>
+        <v>0.00074799999999999997</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>7.4800000000000002e-05</v>
+      </c>
+      <c r="F6" s="1">
+        <v>112.37</v>
+      </c>
+      <c r="G6" s="1">
+        <v>110.29000000000001</v>
+      </c>
+      <c r="H6" s="1">
+        <v>111.06</v>
+      </c>
+      <c r="I6" s="1">
+        <v>108.8</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">

</xml_diff>